<commit_message>
[AV] Work Queen 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/[AV] Work Queen - 3344087854/[AV] Work Queen - 3344087854.xlsx
+++ b/Data/[AV] Work Queen - 3344087854/[AV] Work Queen - 3344087854.xlsx
@@ -5,22 +5,35 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\알티\[AV] Work Queen - 3344087854\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SteamLibrary\steamapps\common\RimWorld\Mods\RMK\Data\[AV] Work Queen - 3344087854\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2618902A-003D-46E0-80CF-257F097C83F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E360054-24ED-42C5-B264-802A2ACEA93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="204">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -64,16 +77,10 @@
     <t>ThingDef+AV_Mech_MinerUrchin.tools.0.label</t>
   </si>
   <si>
-    <t>AV_Mech_MinerUrchin.tools.0.label</t>
-  </si>
-  <si>
     <t>left power claw</t>
   </si>
   <si>
     <t>ThingDef+AV_Mech_MinerUrchin.tools.1.label</t>
-  </si>
-  <si>
-    <t>AV_Mech_MinerUrchin.tools.1.label</t>
   </si>
   <si>
     <t>right power claw</t>
@@ -339,9 +346,6 @@
   </si>
   <si>
     <t>ScenarioDef+AV_CrashlandedMechanitor.scenario.parts.0.text</t>
-  </si>
-  <si>
-    <t>AV_CrashlandedMechanitor.scenario.parts.0.text</t>
   </si>
   <si>
     <t>You awake in your cryptosleep sarcophagi to the sound of sirens and ripping metal. You barely get to your shuttle, where your old companoid mech is already waiting for your commands, before the ship gets torn apart. Your shuttle got damaged in the process and you are forced to crashland at the next best planet.</t>
@@ -540,6 +544,125 @@
   <si>
     <t>이 자동 채움 수량은 정착민들이 이 {0}에 자동으로 배치할 자원의 최대 양을 결정합니다. 자원은 작업 어친을 만드는 데 사용될 수 있습니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AV_CrashlandedMechanitor.scenario.parts.GameStartDialog.text</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AV_Mech_MinerUrchin.tools.left_power_claw.labelNoLocation</t>
+  </si>
+  <si>
+    <t>AV_Mech_MinerUrchin.tools.right_power_claw.label</t>
+  </si>
+  <si>
+    <t>ThinkTreeDef</t>
+  </si>
+  <si>
+    <t>AV_Gestate_Workerqueen.jobString</t>
+  </si>
+  <si>
+    <t>AV_Mech_MinerUrchin.comps.CompMechPowerCell.tooltipOverride</t>
+  </si>
+  <si>
+    <t>AV_Mech_MinerUrchin.tools.right_power_claw.labelNoLocation</t>
+  </si>
+  <si>
+    <t>AV_Mech_HaulerUrchin.comps.CompMechPowerCell.tooltipOverride</t>
+  </si>
+  <si>
+    <t>AV_Mech_HaulerUrchin.tools.head.label</t>
+  </si>
+  <si>
+    <t>AV_Mech_BuilderUrchin.comps.CompMechPowerCell.tooltipOverride</t>
+  </si>
+  <si>
+    <t>AV_Mech_BuilderUrchin.tools.head.label</t>
+  </si>
+  <si>
+    <t>AV_Mech_GrowerUrchin.comps.CompMechPowerCell.tooltipOverride</t>
+  </si>
+  <si>
+    <t>AV_Mech_GrowerUrchin.tools.head.label</t>
+  </si>
+  <si>
+    <t>AV_Mech_CleanerUrchin.comps.CompMechPowerCell.tooltipOverride</t>
+  </si>
+  <si>
+    <t>AV_Mech_CleanerUrchin.tools.head.label</t>
+  </si>
+  <si>
+    <t>AV_MechanitorShuttleCrashed.description</t>
+  </si>
+  <si>
+    <t>AV_FlyingMechanitorShuttleCrashed.description</t>
+  </si>
+  <si>
+    <t>AV_WorkUrchin.thinkRoot.subNodes.1.subNodes.3.subNodes.1.subNodes.0.reportStringOverride</t>
+  </si>
+  <si>
+    <t>Gestating mech.</t>
+  </si>
+  <si>
+    <t>Minurchins have a one-time power source. When the power cell runs out, the mechanoid dies.</t>
+  </si>
+  <si>
+    <t>power claw</t>
+  </si>
+  <si>
+    <t>Carrurchins have a one-time power source. When the power cell runs out, the mechanoid dies.</t>
+  </si>
+  <si>
+    <t>Consturchins have a one-time power source. When the power cell runs out, the mechanoid dies.</t>
+  </si>
+  <si>
+    <t>Agrurchins have a one-time power source. When the power cell runs out, the mechanoid dies.</t>
+  </si>
+  <si>
+    <t>Cleurchins have a one-time power source. When the power cell runs out, the mechanoid dies.</t>
+  </si>
+  <si>
+    <t>A spacer-tech shuttle designed for transit between surface and orbit, or between moons of a planetary system.</t>
+  </si>
+  <si>
+    <t>Patrolling.</t>
+  </si>
+  <si>
+    <t>파워 클로</t>
+  </si>
+  <si>
+    <t>마이너친은 일회용 전원을 가지고 있습니다. 전력 셀이 소진되면 메카노이드가 죽습니다.</t>
+  </si>
+  <si>
+    <t>메크 배양 중…</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>캐리어친은 일회용 전원을 가지고 있습니다. 전력 셀이 소진되면 메카노이드가 죽습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>컨스트러친은 일회용 전원을 가지고 있습니다. 전력 셀이 소진되면 메카노이드가 죽습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>아그러친은 일회용 전원을 가지고 있습니다. 전력 셀이 소진되면 메카노이드가 죽습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>클리어친은 일회용 전원을 가지고 있습니다. 전력 셀이 소진되면 메카노이드가 죽습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지표면과 궤도 사이, 또는 행성계의 위성들 사이를 이동하도록 설계된 우주기술 셔틀.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>순찰 중</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AV_Mech_MinerUrchin.tools.left_power_claw.label</t>
   </si>
 </sst>
 </file>
@@ -894,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -946,7 +1069,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -963,7 +1086,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -974,38 +1097,38 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
@@ -1014,721 +1137,931 @@
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="F25" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="F27" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="F30" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="F33" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="F36" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="F37" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>106</v>
+        <v>167</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="F42" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="F43" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="F44" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E48" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>144</v>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B63" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>